<commit_message>
test case excel modified
</commit_message>
<xml_diff>
--- a/fundamentals_v3/fundamentals_test_cases.xlsx
+++ b/fundamentals_v3/fundamentals_test_cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10808"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shimm\iCloudDrive\Desktop\Study\Summer2021\CPR101\Final Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/myungwooshim/Desktop/Study/Summer2021/CPR101/Final Project/CPRBb02_final_assignment/fundamentals_v3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A20C63-89A5-4F24-B7B4-3A92BBD4CD88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{039A6333-7E97-3946-A648-0F179BFBCC0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCaseMatrix" sheetId="2" r:id="rId1"/>
@@ -56,6 +56,7 @@
             <sz val="12"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> means a positive test expecting a successful result.
 </t>
@@ -75,6 +76,7 @@
             <sz val="12"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> means a negative test to generate a validation message or explore unexpected, undefined behaviours.</t>
         </r>
@@ -85,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="50">
   <si>
     <t>Comments</t>
   </si>
@@ -231,13 +233,46 @@
   <si>
     <t>third input: Good luck to all the group members !</t>
     <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>fundamentals () v3</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>CRP101 Final Project</t>
+  </si>
+  <si>
+    <t>Fundamentals Version 3 is ready</t>
+  </si>
+  <si>
+    <t>Good luck on next semester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thank you </t>
+  </si>
+  <si>
+    <t>New destination string is 'CPR101 Final Project':</t>
+  </si>
+  <si>
+    <t>New destination string is 'Hello':</t>
+  </si>
+  <si>
+    <t>New destination string is Fundamentals Version 3 is ready"</t>
+  </si>
+  <si>
+    <t>New destination string is 'Good luck on next semester':</t>
+  </si>
+  <si>
+    <t>New destination string is 'Thank you':</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -268,6 +303,7 @@
       <sz val="12"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -414,7 +450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -498,6 +534,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -781,24 +820,24 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="20.5" style="7" customWidth="1"/>
     <col min="3" max="3" width="31" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" style="11" customWidth="1"/>
-    <col min="7" max="7" width="28.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="26.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="11" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="13.5" thickBot="1">
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>8</v>
       </c>
@@ -815,7 +854,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="F2" s="15" t="s">
         <v>21</v>
       </c>
@@ -823,7 +862,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="15">
+    <row r="3" spans="1:9" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>6</v>
       </c>
@@ -847,7 +886,7 @@
       </c>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="84" customHeight="1">
+    <row r="4" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>29</v>
       </c>
@@ -869,7 +908,7 @@
       <c r="G4" s="23"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" ht="25.5">
+    <row r="5" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>29</v>
       </c>
@@ -891,7 +930,7 @@
       <c r="G5" s="24"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" ht="25.5">
+    <row r="6" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>28</v>
       </c>
@@ -913,7 +952,7 @@
       <c r="G6" s="23"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" ht="25.5">
+    <row r="7" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>28</v>
       </c>
@@ -935,7 +974,7 @@
       <c r="G7" s="23"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" ht="51">
+    <row r="8" spans="1:9" ht="56" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>28</v>
       </c>
@@ -959,7 +998,7 @@
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" ht="63.75">
+    <row r="9" spans="1:9" ht="70" x14ac:dyDescent="0.15">
       <c r="A9" s="8" t="s">
         <v>27</v>
       </c>
@@ -980,7 +1019,7 @@
       </c>
       <c r="G9" s="27"/>
     </row>
-    <row r="10" spans="1:9" ht="25.5">
+    <row r="10" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A10" s="8" t="s">
         <v>27</v>
       </c>
@@ -1001,7 +1040,7 @@
       </c>
       <c r="G10" s="27"/>
     </row>
-    <row r="11" spans="1:9" ht="25.5">
+    <row r="11" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A11" s="8" t="s">
         <v>26</v>
       </c>
@@ -1022,7 +1061,7 @@
       </c>
       <c r="G11" s="27"/>
     </row>
-    <row r="12" spans="1:9" ht="25.5">
+    <row r="12" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A12" s="8" t="s">
         <v>26</v>
       </c>
@@ -1043,7 +1082,7 @@
       </c>
       <c r="G12" s="27"/>
     </row>
-    <row r="13" spans="1:9" ht="51">
+    <row r="13" spans="1:9" ht="56" x14ac:dyDescent="0.15">
       <c r="A13" s="8" t="s">
         <v>26</v>
       </c>
@@ -1066,7 +1105,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="25.5">
+    <row r="14" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A14" s="8" t="s">
         <v>27</v>
       </c>
@@ -1087,7 +1126,7 @@
       </c>
       <c r="G14" s="28"/>
     </row>
-    <row r="15" spans="1:9" ht="25.5">
+    <row r="15" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A15" s="8" t="s">
         <v>27</v>
       </c>
@@ -1108,7 +1147,7 @@
       </c>
       <c r="G15" s="27"/>
     </row>
-    <row r="16" spans="1:9" ht="25.5">
+    <row r="16" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A16" s="8" t="s">
         <v>26</v>
       </c>
@@ -1129,7 +1168,7 @@
       </c>
       <c r="G16" s="27"/>
     </row>
-    <row r="17" spans="1:7" ht="25.5">
+    <row r="17" spans="1:7" ht="28" x14ac:dyDescent="0.15">
       <c r="A17" s="8" t="s">
         <v>26</v>
       </c>
@@ -1150,7 +1189,7 @@
       </c>
       <c r="G17" s="27"/>
     </row>
-    <row r="18" spans="1:7" ht="25.5">
+    <row r="18" spans="1:7" ht="28" x14ac:dyDescent="0.15">
       <c r="A18" s="8" t="s">
         <v>26</v>
       </c>
@@ -1170,6 +1209,111 @@
         <v>1</v>
       </c>
       <c r="G18" s="27"/>
+    </row>
+    <row r="19" spans="1:7" ht="28" x14ac:dyDescent="0.15">
+      <c r="A19" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="27"/>
+    </row>
+    <row r="20" spans="1:7" ht="28" x14ac:dyDescent="0.15">
+      <c r="A20" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G20" s="27"/>
+    </row>
+    <row r="21" spans="1:7" ht="42" x14ac:dyDescent="0.15">
+      <c r="A21" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G21" s="27"/>
+    </row>
+    <row r="22" spans="1:7" ht="28" x14ac:dyDescent="0.15">
+      <c r="A22" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G22" s="27"/>
+    </row>
+    <row r="23" spans="1:7" ht="28" x14ac:dyDescent="0.15">
+      <c r="A23" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23" s="27"/>
     </row>
   </sheetData>
   <dataConsolidate/>

</xml_diff>